<commit_message>
improved global design and cleaned up code
</commit_message>
<xml_diff>
--- a/digital-region/src/test/resources/TestData/Itineraires.xlsx
+++ b/digital-region/src/test/resources/TestData/Itineraires.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t>ID</t>
   </si>
@@ -72,13 +72,16 @@
     <t>St-Malo</t>
   </si>
   <si>
-    <t>29/11/2017</t>
-  </si>
-  <si>
     <t>30/11/2017</t>
   </si>
   <si>
     <t>18h</t>
+  </si>
+  <si>
+    <t>01/12/2017</t>
+  </si>
+  <si>
+    <t>19h</t>
   </si>
 </sst>
 </file>
@@ -421,7 +424,7 @@
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -499,7 +502,7 @@
         <v>18</v>
       </c>
       <c r="F2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H2" t="s">
         <v>13</v>
@@ -511,10 +514,10 @@
         <v>15</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="L2">
-        <v>18</v>
+        <v>20</v>
+      </c>
+      <c r="L2" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added new data set for testings purposes
</commit_message>
<xml_diff>
--- a/digital-region/src/test/resources/TestData/Itineraires.xlsx
+++ b/digital-region/src/test/resources/TestData/Itineraires.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
   <si>
     <t>ID</t>
   </si>
@@ -82,6 +82,15 @@
   </si>
   <si>
     <t>19h</t>
+  </si>
+  <si>
+    <t>05/12/2017</t>
+  </si>
+  <si>
+    <t>12h</t>
+  </si>
+  <si>
+    <t>13h</t>
   </si>
 </sst>
 </file>
@@ -421,10 +430,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -520,8 +529,44 @@
         <v>21</v>
       </c>
     </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J3" t="s">
+        <v>15</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L3" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>